<commit_message>
Cite data on forced outage rates
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587F779-3CDB-4264-A4FE-7C47012C706C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8552F65-6217-4954-869B-9B7FB9ABC223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>natural gas nonpeaker</t>
   </si>
@@ -118,9 +118,6 @@
     <t>MCF Maximum Capacity Factor</t>
   </si>
   <si>
-    <t>None needed</t>
-  </si>
-  <si>
     <t>This represents the maximum capacity factor a plant type can achieve</t>
   </si>
   <si>
@@ -130,7 +127,19 @@
     <t>a 5% penalty to represent that plants are not typically available 100% of the</t>
   </si>
   <si>
-    <t>year due to factors like plant maintenance.</t>
+    <t>The Myth of the 24/7/365 Power Plant</t>
+  </si>
+  <si>
+    <t>National Resources Defense Council</t>
+  </si>
+  <si>
+    <t>https://www.nrdc.org/bio/rachel-fakhry/myth-247365-power-plant</t>
+  </si>
+  <si>
+    <t>year due to factors like plant maintenance, based on the value for gas plants</t>
+  </si>
+  <si>
+    <t>in the NRDC source above. For coal, we apply a 15% penalty based on NRDC.</t>
   </si>
 </sst>
 </file>
@@ -279,7 +288,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -295,13 +304,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -723,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,56 +747,88 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="2">
+        <v>2019</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A22" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Summer, Winter"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{F347B8A5-4293-4AF0-8AF8-8B455D7F79DF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -806,7 +840,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,7 +861,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="3">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="C2" s="3"/>
     </row>
@@ -854,7 +888,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
       <c r="C5" s="3"/>
     </row>

</xml_diff>

<commit_message>
Fix label in elec/MCF
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\elec\MCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4443B04D-F45B-41B0-9630-2317F5CDFE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C22BA7F-3307-47E6-8D94-A6FFE854A00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7455" yWindow="960" windowWidth="33780" windowHeight="21990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -55,9 +55,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>natural gas nonpeaker</t>
-  </si>
-  <si>
     <t>nuclear</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>hydrogen</t>
+  </si>
+  <si>
+    <t>natural gas peaker</t>
   </si>
 </sst>
 </file>
@@ -745,9 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -759,7 +757,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -767,10 +765,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1"/>
       <c r="H3" s="1"/>
@@ -786,7 +784,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1"/>
       <c r="H5" s="1"/>
@@ -794,7 +792,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1"/>
       <c r="H6" s="1"/>
@@ -804,36 +802,36 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -857,9 +855,7 @@
   </sheetPr>
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -869,14 +865,14 @@
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>0.85</v>
@@ -885,7 +881,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>0.95</v>
@@ -894,7 +890,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0.95</v>
@@ -903,7 +899,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="3">
         <v>0.91</v>
@@ -912,7 +908,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -921,7 +917,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -930,7 +926,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -939,7 +935,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -948,7 +944,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="3">
         <v>0.95</v>
@@ -957,7 +953,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>0.95</v>
@@ -966,7 +962,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3">
         <v>0.95</v>
@@ -975,7 +971,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3">
         <v>0.95</v>
@@ -984,7 +980,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" s="3">
         <v>0.95</v>
@@ -993,7 +989,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -1002,7 +998,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>0.95</v>
@@ -1011,7 +1007,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>0.95</v>
@@ -1020,7 +1016,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>0.95</v>
@@ -1029,7 +1025,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="3">
         <f>B2</f>
@@ -1038,7 +1034,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="3">
         <f>B4</f>
@@ -1047,7 +1043,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="3">
         <f>B10</f>
@@ -1056,7 +1052,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="3">
         <f>B14</f>
@@ -1065,7 +1061,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="3">
         <f>B5</f>
@@ -1074,7 +1070,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="3">
         <f>B4</f>

</xml_diff>

<commit_message>
Edits to help move historical generation closer to observed values
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\MCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF5E761-3510-4551-BBBD-14D4B578101B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8334E663-49B3-49C3-93A5-0BC636FA8FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -758,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +870,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>

<commit_message>
Revert "Edits to help move historical generation closer to observed values"
This reverts commit 8cafccbd54ecfbcc6e28a3572fe2ca9a4a47bfc7.
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8334E663-49B3-49C3-93A5-0BC636FA8FC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF5E761-3510-4551-BBBD-14D4B578101B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -758,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -870,7 +870,7 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -928,7 +928,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="3">
-        <v>0.85</v>
+        <v>0.95</v>
       </c>
       <c r="C6" s="3"/>
     </row>

</xml_diff>

<commit_message>
Make MCF and RAF variables time series
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\elec\MCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF5E761-3510-4551-BBBD-14D4B578101B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA46C6EB-58F3-4682-99A9-C7621CA2B7C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="23640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -316,7 +316,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -329,9 +329,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -868,10 +865,10 @@
   <sheetPr>
     <tabColor rgb="FF002060"/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AE25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,167 +877,1717 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="5">
+        <v>2021</v>
+      </c>
+      <c r="C1" s="5">
+        <v>2022</v>
+      </c>
+      <c r="D1" s="5">
+        <v>2023</v>
+      </c>
+      <c r="E1" s="5">
+        <v>2024</v>
+      </c>
+      <c r="F1" s="5">
+        <v>2025</v>
+      </c>
+      <c r="G1" s="5">
+        <v>2026</v>
+      </c>
+      <c r="H1" s="5">
+        <v>2027</v>
+      </c>
+      <c r="I1" s="5">
+        <v>2028</v>
+      </c>
+      <c r="J1" s="5">
+        <v>2029</v>
+      </c>
+      <c r="K1" s="5">
+        <v>2030</v>
+      </c>
+      <c r="L1" s="5">
+        <v>2031</v>
+      </c>
+      <c r="M1" s="5">
+        <v>2032</v>
+      </c>
+      <c r="N1" s="5">
+        <v>2033</v>
+      </c>
+      <c r="O1" s="5">
+        <v>2034</v>
+      </c>
+      <c r="P1" s="5">
+        <v>2035</v>
+      </c>
+      <c r="Q1" s="5">
+        <v>2036</v>
+      </c>
+      <c r="R1" s="5">
+        <v>2037</v>
+      </c>
+      <c r="S1" s="5">
+        <v>2038</v>
+      </c>
+      <c r="T1" s="5">
+        <v>2039</v>
+      </c>
+      <c r="U1" s="5">
+        <v>2040</v>
+      </c>
+      <c r="V1" s="5">
+        <v>2041</v>
+      </c>
+      <c r="W1" s="5">
+        <v>2042</v>
+      </c>
+      <c r="X1" s="5">
+        <v>2043</v>
+      </c>
+      <c r="Y1" s="5">
+        <v>2044</v>
+      </c>
+      <c r="Z1" s="5">
+        <v>2045</v>
+      </c>
+      <c r="AA1" s="5">
+        <v>2046</v>
+      </c>
+      <c r="AB1" s="5">
+        <v>2047</v>
+      </c>
+      <c r="AC1" s="5">
+        <v>2048</v>
+      </c>
+      <c r="AD1" s="5">
+        <v>2049</v>
+      </c>
+      <c r="AE1" s="5">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>0.85</v>
       </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="O2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="P2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="R2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="S2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="T2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="U2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="V2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="W2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="X2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="Z2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="AA2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="AB2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="AC2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="AD2" s="3">
+        <v>0.85</v>
+      </c>
+      <c r="AE2" s="3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="3">
         <v>0.95</v>
       </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="3">
         <v>0.95</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3">
         <v>0.91</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="R5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="T5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>0.91</v>
+      </c>
+      <c r="AE5" s="3">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="3">
         <v>0.95</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE6" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>0</v>
+      </c>
+      <c r="P7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0</v>
+      </c>
+      <c r="S7" s="3">
+        <v>0</v>
+      </c>
+      <c r="T7" s="3">
+        <v>0</v>
+      </c>
+      <c r="U7" s="3">
+        <v>0</v>
+      </c>
+      <c r="V7" s="3">
+        <v>0</v>
+      </c>
+      <c r="W7" s="3">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="M8" s="3">
+        <v>0</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>0</v>
+      </c>
+      <c r="P8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3">
+        <v>0</v>
+      </c>
+      <c r="S8" s="3">
+        <v>0</v>
+      </c>
+      <c r="T8" s="3">
+        <v>0</v>
+      </c>
+      <c r="U8" s="3">
+        <v>0</v>
+      </c>
+      <c r="V8" s="3">
+        <v>0</v>
+      </c>
+      <c r="W8" s="3">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="M9" s="3">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>0</v>
+      </c>
+      <c r="P9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3">
+        <v>0</v>
+      </c>
+      <c r="S9" s="3">
+        <v>0</v>
+      </c>
+      <c r="T9" s="3">
+        <v>0</v>
+      </c>
+      <c r="U9" s="3">
+        <v>0</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0</v>
+      </c>
+      <c r="W9" s="3">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3">
         <v>0.95</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE10" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="3">
         <v>0.95</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="3">
         <v>0.95</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="3">
         <v>0.95</v>
       </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE13" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="3">
         <v>0.95</v>
       </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE14" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
       </c>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0</v>
+      </c>
+      <c r="R15" s="3">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="3">
+        <v>0</v>
+      </c>
+      <c r="U15" s="3">
+        <v>0</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="3">
         <v>0.95</v>
       </c>
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE16" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>0.95</v>
       </c>
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE17" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="3">
         <v>0.95</v>
       </c>
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="L18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="N18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="O18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="P18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="R18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="T18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="U18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Y18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>0.95</v>
+      </c>
+      <c r="AE18" s="3">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1048,8 +2595,124 @@
         <f>B2</f>
         <v>0.85</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <f t="shared" ref="C19:AE19" si="0">C2</f>
+        <v>0.85</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="O19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="P19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="R19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="S19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="T19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="U19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="V19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="W19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="X19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="Y19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="Z19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="AA19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="AB19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="AC19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="AD19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+      <c r="AE19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1057,8 +2720,124 @@
         <f>B4</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <f t="shared" ref="C20:AE20" si="1">C4</f>
+        <v>0.95</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="M20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="O20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="P20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="R20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="S20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="T20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="U20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="V20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="W20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="X20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="Y20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="Z20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="AA20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="AB20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="AC20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="AD20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+      <c r="AE20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1066,8 +2845,124 @@
         <f>B10</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <f t="shared" ref="C21:AE21" si="2">C10</f>
+        <v>0.95</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="G21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="J21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="M21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="O21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="P21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="R21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="S21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="T21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="U21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="V21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="W21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="X21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="Y21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="Z21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="AA21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="AB21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="AC21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="AD21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+      <c r="AE21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -1075,8 +2970,124 @@
         <f>B14</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <f t="shared" ref="C22:AE22" si="3">C14</f>
+        <v>0.95</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="J22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="M22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="O22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="P22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="R22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="S22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="T22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="U22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="V22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="W22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="X22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="Y22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="Z22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="AA22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="AB22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="AC22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="AD22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+      <c r="AE22" s="3">
+        <f t="shared" si="3"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1084,22 +3095,370 @@
         <f>B5</f>
         <v>0.91</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="C23" s="3">
+        <f t="shared" ref="C23:AE23" si="4">C5</f>
+        <v>0.91</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="J23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="M23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="O23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="P23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="R23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="S23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="T23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="U23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="V23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="W23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="X23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="Y23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="Z23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="AA23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="AB23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="AC23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="AD23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+      <c r="AE23" s="3">
+        <f t="shared" si="4"/>
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B24" s="3">
         <f>B4</f>
         <v>0.95</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
+      <c r="C24" s="3">
+        <f t="shared" ref="C24:AE24" si="5">C4</f>
+        <v>0.95</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="J24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="M24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="N24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="O24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="P24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="R24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="S24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="T24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="U24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="V24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="W24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="X24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="Y24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="Z24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="AA24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="AB24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="AC24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="AD24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+      <c r="AE24" s="3">
+        <f t="shared" si="5"/>
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="3">
         <f>B4</f>
+        <v>0.95</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" ref="C25:AE25" si="6">C4</f>
+        <v>0.95</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="J25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="M25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="N25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="O25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="P25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="R25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="S25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="T25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="U25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="V25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="W25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="X25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="Y25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="Z25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="AA25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="AB25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="AC25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="AD25" s="3">
+        <f t="shared" si="6"/>
+        <v>0.95</v>
+      </c>
+      <c r="AE25" s="3">
+        <f t="shared" si="6"/>
         <v>0.95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Remove additional 111 rule customizations
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B64DA94-7A2B-46EC-A4E2-18C6018E050D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34BB8B4-A134-43E7-BBB4-1F6BF5186A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -1851,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8761,8 +8761,8 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:AE2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8871,124 +8871,94 @@
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <f>'Coal Calculations'!B9</f>
         <v>0.85</v>
       </c>
       <c r="C2" s="3">
-        <f>'Coal Calculations'!C9</f>
         <v>0.85</v>
       </c>
       <c r="D2" s="3">
-        <f>'Coal Calculations'!D9</f>
         <v>0.85</v>
       </c>
       <c r="E2" s="3">
-        <f>'Coal Calculations'!E9</f>
         <v>0.85</v>
       </c>
       <c r="F2" s="3">
-        <f>'Coal Calculations'!F9</f>
         <v>0.85</v>
       </c>
       <c r="G2" s="3">
-        <f>'Coal Calculations'!G9</f>
         <v>0.85</v>
       </c>
       <c r="H2" s="3">
-        <f>'Coal Calculations'!H9</f>
         <v>0.85</v>
       </c>
       <c r="I2" s="3">
-        <f>'Coal Calculations'!I9</f>
         <v>0.85</v>
       </c>
       <c r="J2" s="3">
-        <f>'Coal Calculations'!J9</f>
         <v>0.85</v>
       </c>
       <c r="K2" s="3">
-        <f>'Coal Calculations'!K9</f>
         <v>0.85</v>
       </c>
       <c r="L2" s="3">
-        <f>'Coal Calculations'!L9</f>
         <v>0.85</v>
       </c>
       <c r="M2" s="3">
-        <f>'Coal Calculations'!M9</f>
         <v>0.85</v>
       </c>
       <c r="N2" s="3">
-        <f>'Coal Calculations'!N9</f>
         <v>0.85</v>
       </c>
       <c r="O2" s="3">
-        <f>'Coal Calculations'!O9</f>
         <v>0.85</v>
       </c>
       <c r="P2" s="3">
-        <f>'Coal Calculations'!P9</f>
         <v>0.85</v>
       </c>
       <c r="Q2" s="3">
-        <f>'Coal Calculations'!Q9</f>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R2" s="3">
-        <f>'Coal Calculations'!R9</f>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S2" s="3">
-        <f>'Coal Calculations'!S9</f>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T2" s="3">
-        <f>'Coal Calculations'!T9</f>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U2" s="3">
-        <f>'Coal Calculations'!U9</f>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V2" s="3">
-        <f>'Coal Calculations'!V9</f>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W2" s="3">
-        <f>'Coal Calculations'!W9</f>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X2" s="3">
-        <f>'Coal Calculations'!X9</f>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y2" s="3">
-        <f>'Coal Calculations'!Y9</f>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z2" s="3">
-        <f>'Coal Calculations'!Z9</f>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA2" s="3">
-        <f>'Coal Calculations'!AA9</f>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB2" s="3">
-        <f>'Coal Calculations'!AB9</f>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC2" s="3">
-        <f>'Coal Calculations'!AC9</f>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD2" s="3">
-        <f>'Coal Calculations'!AD9</f>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE2" s="3">
-        <f>'Coal Calculations'!AE9</f>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -10577,63 +10547,63 @@
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="0"/>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="0"/>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="0"/>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T19" s="3">
         <f t="shared" si="0"/>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U19" s="3">
         <f t="shared" si="0"/>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="0"/>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W19" s="3">
         <f t="shared" si="0"/>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X19" s="3">
         <f t="shared" si="0"/>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y19" s="3">
         <f t="shared" si="0"/>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z19" s="3">
         <f t="shared" si="0"/>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA19" s="3">
         <f t="shared" si="0"/>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB19" s="3">
         <f t="shared" si="0"/>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC19" s="3">
         <f t="shared" si="0"/>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD19" s="3">
         <f t="shared" si="0"/>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE19" s="3">
         <f t="shared" si="0"/>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Calibration run with ATB 2023 data that removes 111 rules
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8901C8-0A08-45FE-BA2D-BF915959C34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692CDF7C-DDC3-4828-8489-9260C0722EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -1851,16 +1851,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" customWidth="1"/>
-    <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.54296875" customWidth="1"/>
-    <col min="8" max="8" width="53.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2024,11 +2024,11 @@
       <selection activeCell="C33" sqref="C33:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.26953125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="65.28515625" style="58" customWidth="1"/>
     <col min="2" max="2" width="2" style="58" customWidth="1"/>
-    <col min="3" max="8" width="8.453125" style="9" customWidth="1"/>
+    <col min="3" max="8" width="8.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2040,7 +2040,7 @@
       <c r="F1" s="8"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:14" ht="25">
+    <row r="2" spans="1:14" ht="26.25">
       <c r="A2" s="102" t="s">
         <v>35</v>
       </c>
@@ -2084,7 +2084,7 @@
       <c r="F5" s="8"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:14" ht="15.5">
+    <row r="6" spans="1:14" ht="15.75">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
@@ -2113,7 +2113,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.5" thickBot="1">
+    <row r="10" spans="1:14" ht="18.75" thickBot="1">
       <c r="A10" s="15" t="s">
         <v>40</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="J14" s="37"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15" s="38" t="s">
         <v>45</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="J15" s="37"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="43"/>
@@ -2300,7 +2300,7 @@
       <c r="G16" s="43"/>
       <c r="H16" s="44"/>
     </row>
-    <row r="17" spans="1:10" ht="18.5" thickBot="1">
+    <row r="17" spans="1:10" ht="18.75" thickBot="1">
       <c r="A17" s="15" t="s">
         <v>46</v>
       </c>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="J17" s="19"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="45" t="s">
         <v>47</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="50"/>
@@ -2366,7 +2366,7 @@
       <c r="G19" s="50"/>
       <c r="H19" s="51"/>
     </row>
-    <row r="20" spans="1:10" ht="18.5" thickBot="1">
+    <row r="20" spans="1:10" ht="18.75" thickBot="1">
       <c r="A20" s="15" t="s">
         <v>48</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="J30" s="54"/>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
       <c r="A31" s="61" t="s">
         <v>59</v>
       </c>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="J31" s="54"/>
     </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="65"/>
@@ -2667,7 +2667,7 @@
       <c r="G32" s="65"/>
       <c r="H32" s="65"/>
     </row>
-    <row r="33" spans="1:10" ht="18.5" thickBot="1">
+    <row r="33" spans="1:10" ht="18.75" thickBot="1">
       <c r="A33" s="15" t="s">
         <v>60</v>
       </c>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="J37" s="68"/>
     </row>
-    <row r="38" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="38" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A38" s="57" t="s">
         <v>65</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="J38" s="68"/>
     </row>
-    <row r="39" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="39" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A39" s="59" t="s">
         <v>66</v>
       </c>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="J39" s="68"/>
     </row>
-    <row r="40" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="40" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A40" s="57" t="s">
         <v>67</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="J40" s="68"/>
     </row>
-    <row r="41" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="41" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A41" s="59" t="s">
         <v>68</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="J42" s="68"/>
     </row>
-    <row r="43" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="43" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A43" s="59" t="s">
         <v>70</v>
       </c>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="J43" s="68"/>
     </row>
-    <row r="44" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="44" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A44" s="57" t="s">
         <v>71</v>
       </c>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="J44" s="68"/>
     </row>
-    <row r="45" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="45" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A45" s="59" t="s">
         <v>72</v>
       </c>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="J48" s="68"/>
     </row>
-    <row r="49" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="49" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A49" s="59" t="s">
         <v>76</v>
       </c>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="J49" s="68"/>
     </row>
-    <row r="50" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="50" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A50" s="57" t="s">
         <v>77</v>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="J53" s="68"/>
     </row>
-    <row r="54" spans="1:10" ht="15" thickBot="1">
+    <row r="54" spans="1:10" ht="15.75" thickBot="1">
       <c r="A54" s="76" t="s">
         <v>81</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J54" s="68"/>
     </row>
-    <row r="55" spans="1:10" ht="15.5" thickTop="1" thickBot="1">
+    <row r="55" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="66"/>
@@ -3289,7 +3289,7 @@
       <c r="G55" s="66"/>
       <c r="H55" s="66"/>
     </row>
-    <row r="56" spans="1:10" ht="18.5" thickBot="1">
+    <row r="56" spans="1:10" ht="18.75" thickBot="1">
       <c r="A56" s="15" t="s">
         <v>82</v>
       </c>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="J60" s="81"/>
     </row>
-    <row r="61" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="61" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A61" s="57" t="s">
         <v>65</v>
       </c>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="J61" s="81"/>
     </row>
-    <row r="62" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="62" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A62" s="59" t="s">
         <v>66</v>
       </c>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="J62" s="81"/>
     </row>
-    <row r="63" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="63" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A63" s="57" t="s">
         <v>67</v>
       </c>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="J64" s="81"/>
     </row>
-    <row r="65" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="65" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A65" s="57" t="s">
         <v>70</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="J65" s="81"/>
     </row>
-    <row r="66" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="66" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A66" s="82" t="s">
         <v>71</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="J66" s="81"/>
     </row>
-    <row r="67" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="67" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A67" s="57" t="s">
         <v>72</v>
       </c>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="J70" s="81"/>
     </row>
-    <row r="71" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="71" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A71" s="57" t="s">
         <v>76</v>
       </c>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J71" s="81"/>
     </row>
-    <row r="72" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="72" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A72" s="83" t="s">
         <v>77</v>
       </c>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J74" s="81"/>
     </row>
-    <row r="75" spans="1:10" ht="15" thickBot="1">
+    <row r="75" spans="1:10" ht="15.75" thickBot="1">
       <c r="A75" s="84" t="s">
         <v>81</v>
       </c>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="J75" s="81"/>
     </row>
-    <row r="76" spans="1:10" ht="15" thickBot="1">
+    <row r="76" spans="1:10" ht="15.75" thickBot="1">
       <c r="A76" s="38"/>
       <c r="B76" s="39"/>
       <c r="C76" s="88"/>
@@ -3861,7 +3861,7 @@
       <c r="I76" s="88"/>
       <c r="J76" s="81"/>
     </row>
-    <row r="77" spans="1:10" ht="18.5" thickBot="1">
+    <row r="77" spans="1:10" ht="18.75" thickBot="1">
       <c r="A77" s="15" t="s">
         <v>83</v>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="J81" s="81"/>
     </row>
-    <row r="82" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="82" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A82" s="57" t="s">
         <v>65</v>
       </c>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="J82" s="81"/>
     </row>
-    <row r="83" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="83" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A83" s="59" t="s">
         <v>66</v>
       </c>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="J83" s="81"/>
     </row>
-    <row r="84" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="84" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A84" s="57" t="s">
         <v>67</v>
       </c>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="J85" s="81"/>
     </row>
-    <row r="86" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="86" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A86" s="57" t="s">
         <v>70</v>
       </c>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="J86" s="81"/>
     </row>
-    <row r="87" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="87" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A87" s="82" t="s">
         <v>71</v>
       </c>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="J87" s="81"/>
     </row>
-    <row r="88" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="88" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A88" s="57" t="s">
         <v>72</v>
       </c>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="J91" s="81"/>
     </row>
-    <row r="92" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="92" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A92" s="57" t="s">
         <v>76</v>
       </c>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="J92" s="81"/>
     </row>
-    <row r="93" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="93" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A93" s="83" t="s">
         <v>77</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="J95" s="81"/>
     </row>
-    <row r="96" spans="1:10" ht="15" thickBot="1">
+    <row r="96" spans="1:10" ht="15.75" thickBot="1">
       <c r="A96" s="84" t="s">
         <v>81</v>
       </c>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J96" s="81"/>
     </row>
-    <row r="97" spans="1:10" ht="15" thickBot="1">
+    <row r="97" spans="1:10" ht="15.75" thickBot="1">
       <c r="A97" s="21"/>
       <c r="B97" s="21"/>
       <c r="C97" s="66"/>
@@ -4431,7 +4431,7 @@
       <c r="G97" s="66"/>
       <c r="H97" s="66"/>
     </row>
-    <row r="98" spans="1:10" ht="18.5" thickBot="1">
+    <row r="98" spans="1:10" ht="18.75" thickBot="1">
       <c r="A98" s="15" t="s">
         <v>84</v>
       </c>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="J110" s="68"/>
     </row>
-    <row r="111" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="111" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A111" s="58" t="s">
         <v>97</v>
       </c>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="J111" s="68"/>
     </row>
-    <row r="112" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="112" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A112" s="60" t="s">
         <v>98</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="J112" s="68"/>
     </row>
-    <row r="113" spans="1:10" s="73" customFormat="1" thickBot="1">
+    <row r="113" spans="1:10" s="73" customFormat="1" ht="15.75" thickBot="1">
       <c r="A113" s="84" t="s">
         <v>81</v>
       </c>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="J113" s="68"/>
     </row>
-    <row r="114" spans="1:10" s="73" customFormat="1" ht="15" thickBot="1">
+    <row r="114" spans="1:10" s="73" customFormat="1" ht="15.75" thickBot="1">
       <c r="A114" s="58"/>
       <c r="B114" s="58"/>
       <c r="C114" s="66"/>
@@ -4884,7 +4884,7 @@
       <c r="I114"/>
       <c r="J114" s="68"/>
     </row>
-    <row r="115" spans="1:10" s="73" customFormat="1" ht="18.5" thickBot="1">
+    <row r="115" spans="1:10" s="73" customFormat="1" ht="18.75" thickBot="1">
       <c r="A115" s="15" t="s">
         <v>99</v>
       </c>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="J115" s="68"/>
     </row>
-    <row r="116" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="116" spans="1:10" s="73" customFormat="1">
       <c r="A116" s="20" t="s">
         <v>61</v>
       </c>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="J117" s="92"/>
     </row>
-    <row r="118" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="118" spans="1:10" s="73" customFormat="1">
       <c r="A118" s="57" t="s">
         <v>63</v>
       </c>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="J118" s="68"/>
     </row>
-    <row r="119" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="119" spans="1:10" s="73" customFormat="1">
       <c r="A119" s="59" t="s">
         <v>100</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="J119" s="68"/>
     </row>
-    <row r="120" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="120" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A120" s="57" t="s">
         <v>64</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="J124" s="68"/>
     </row>
-    <row r="125" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="125" spans="1:10" s="73" customFormat="1">
       <c r="A125" s="27" t="s">
         <v>69</v>
       </c>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="J125" s="68"/>
     </row>
-    <row r="126" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="126" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A126" s="57" t="s">
         <v>101</v>
       </c>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="J136" s="68"/>
     </row>
-    <row r="137" spans="1:10" ht="15" thickBot="1">
+    <row r="137" spans="1:10" ht="15.75" thickBot="1">
       <c r="A137" s="93" t="s">
         <v>81</v>
       </c>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="J137" s="68"/>
     </row>
-    <row r="138" spans="1:10" ht="15.5" thickTop="1" thickBot="1">
+    <row r="138" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A138" s="21"/>
       <c r="B138" s="21"/>
       <c r="C138" s="66"/>
@@ -5531,7 +5531,7 @@
       <c r="H138" s="66"/>
       <c r="J138" s="68"/>
     </row>
-    <row r="139" spans="1:10" ht="18.5" thickBot="1">
+    <row r="139" spans="1:10" ht="18.75" thickBot="1">
       <c r="A139" s="15" t="s">
         <v>102</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="H155" s="69"/>
       <c r="I155" s="70"/>
     </row>
-    <row r="156" spans="1:10" ht="15" thickBot="1">
+    <row r="156" spans="1:10" ht="15.75" thickBot="1">
       <c r="A156" s="38" t="s">
         <v>115</v>
       </c>
@@ -6002,12 +6002,12 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.5" thickBot="1">
+    <row r="1" spans="1:31" ht="18.75" thickBot="1">
       <c r="B1" s="17">
         <v>2028</v>
       </c>
@@ -6367,7 +6367,7 @@
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -8761,17 +8761,17 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="29">
+    <row r="1" spans="1:31" ht="30">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -8871,124 +8871,94 @@
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <f>'Coal Calculations'!B9</f>
         <v>0.85</v>
       </c>
       <c r="C2" s="3">
-        <f>'Coal Calculations'!C9</f>
         <v>0.85</v>
       </c>
       <c r="D2" s="3">
-        <f>'Coal Calculations'!D9</f>
         <v>0.85</v>
       </c>
       <c r="E2" s="3">
-        <f>'Coal Calculations'!E9</f>
         <v>0.85</v>
       </c>
       <c r="F2" s="3">
-        <f>'Coal Calculations'!F9</f>
         <v>0.85</v>
       </c>
       <c r="G2" s="3">
-        <f>'Coal Calculations'!G9</f>
         <v>0.85</v>
       </c>
       <c r="H2" s="3">
-        <f>'Coal Calculations'!H9</f>
         <v>0.85</v>
       </c>
       <c r="I2" s="3">
-        <f>'Coal Calculations'!I9</f>
         <v>0.85</v>
       </c>
       <c r="J2" s="3">
-        <f>'Coal Calculations'!J9</f>
         <v>0.85</v>
       </c>
       <c r="K2" s="3">
-        <f>'Coal Calculations'!K9</f>
         <v>0.85</v>
       </c>
       <c r="L2" s="3">
-        <f>'Coal Calculations'!L9</f>
         <v>0.85</v>
       </c>
       <c r="M2" s="3">
-        <f>'Coal Calculations'!M9</f>
         <v>0.85</v>
       </c>
       <c r="N2" s="3">
-        <f>'Coal Calculations'!N9</f>
         <v>0.85</v>
       </c>
       <c r="O2" s="3">
-        <f>'Coal Calculations'!O9</f>
         <v>0.85</v>
       </c>
       <c r="P2" s="3">
-        <f>'Coal Calculations'!P9</f>
         <v>0.85</v>
       </c>
       <c r="Q2" s="3">
-        <f>'Coal Calculations'!Q9</f>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R2" s="3">
-        <f>'Coal Calculations'!R9</f>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S2" s="3">
-        <f>'Coal Calculations'!S9</f>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T2" s="3">
-        <f>'Coal Calculations'!T9</f>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U2" s="3">
-        <f>'Coal Calculations'!U9</f>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V2" s="3">
-        <f>'Coal Calculations'!V9</f>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W2" s="3">
-        <f>'Coal Calculations'!W9</f>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X2" s="3">
-        <f>'Coal Calculations'!X9</f>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y2" s="3">
-        <f>'Coal Calculations'!Y9</f>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z2" s="3">
-        <f>'Coal Calculations'!Z9</f>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA2" s="3">
-        <f>'Coal Calculations'!AA9</f>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB2" s="3">
-        <f>'Coal Calculations'!AB9</f>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC2" s="3">
-        <f>'Coal Calculations'!AC9</f>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD2" s="3">
-        <f>'Coal Calculations'!AD9</f>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE2" s="3">
-        <f>'Coal Calculations'!AE9</f>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -10577,63 +10547,63 @@
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="0"/>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="0"/>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="0"/>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T19" s="3">
         <f t="shared" si="0"/>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U19" s="3">
         <f t="shared" si="0"/>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="0"/>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W19" s="3">
         <f t="shared" si="0"/>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X19" s="3">
         <f t="shared" si="0"/>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y19" s="3">
         <f t="shared" si="0"/>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z19" s="3">
         <f t="shared" si="0"/>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA19" s="3">
         <f t="shared" si="0"/>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB19" s="3">
         <f t="shared" si="0"/>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC19" s="3">
         <f t="shared" si="0"/>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD19" s="3">
         <f t="shared" si="0"/>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE19" s="3">
         <f t="shared" si="0"/>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="1:31">

</xml_diff>

<commit_message>
Undo 111 coal capacity factor customizations
</commit_message>
<xml_diff>
--- a/InputData/elec/MCF/Maximum Capacity Factor.xlsx
+++ b/InputData/elec/MCF/Maximum Capacity Factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\MCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8901C8-0A08-45FE-BA2D-BF915959C34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4EA080-2835-46E2-ACAA-C8B525FFB4D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="12" r:id="rId1"/>
@@ -1851,16 +1851,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" customWidth="1"/>
-    <col min="2" max="2" width="50.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.54296875" customWidth="1"/>
-    <col min="8" max="8" width="53.7265625" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" customWidth="1"/>
+    <col min="8" max="8" width="53.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2024,11 +2024,11 @@
       <selection activeCell="C33" sqref="C33:I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="65.26953125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="65.28515625" style="58" customWidth="1"/>
     <col min="2" max="2" width="2" style="58" customWidth="1"/>
-    <col min="3" max="8" width="8.453125" style="9" customWidth="1"/>
+    <col min="3" max="8" width="8.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2040,7 +2040,7 @@
       <c r="F1" s="8"/>
       <c r="G1"/>
     </row>
-    <row r="2" spans="1:14" ht="25">
+    <row r="2" spans="1:14" ht="26.25">
       <c r="A2" s="102" t="s">
         <v>35</v>
       </c>
@@ -2084,7 +2084,7 @@
       <c r="F5" s="8"/>
       <c r="G5"/>
     </row>
-    <row r="6" spans="1:14" ht="15.5">
+    <row r="6" spans="1:14" ht="15.75">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
@@ -2113,7 +2113,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="18.5" thickBot="1">
+    <row r="10" spans="1:14" ht="18.75" thickBot="1">
       <c r="A10" s="15" t="s">
         <v>40</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="J14" s="37"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1">
+    <row r="15" spans="1:14" ht="15.75" thickBot="1">
       <c r="A15" s="38" t="s">
         <v>45</v>
       </c>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="J15" s="37"/>
     </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1">
+    <row r="16" spans="1:14" ht="15.75" thickBot="1">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="43"/>
@@ -2300,7 +2300,7 @@
       <c r="G16" s="43"/>
       <c r="H16" s="44"/>
     </row>
-    <row r="17" spans="1:10" ht="18.5" thickBot="1">
+    <row r="17" spans="1:10" ht="18.75" thickBot="1">
       <c r="A17" s="15" t="s">
         <v>46</v>
       </c>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="J17" s="19"/>
     </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="45" t="s">
         <v>47</v>
       </c>
@@ -2356,7 +2356,7 @@
       </c>
       <c r="J18" s="49"/>
     </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1">
       <c r="A19" s="21"/>
       <c r="B19" s="21"/>
       <c r="C19" s="50"/>
@@ -2366,7 +2366,7 @@
       <c r="G19" s="50"/>
       <c r="H19" s="51"/>
     </row>
-    <row r="20" spans="1:10" ht="18.5" thickBot="1">
+    <row r="20" spans="1:10" ht="18.75" thickBot="1">
       <c r="A20" s="15" t="s">
         <v>48</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
       <c r="J30" s="54"/>
     </row>
-    <row r="31" spans="1:10" ht="15" thickBot="1">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
       <c r="A31" s="61" t="s">
         <v>59</v>
       </c>
@@ -2657,7 +2657,7 @@
       </c>
       <c r="J31" s="54"/>
     </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1">
       <c r="A32" s="21"/>
       <c r="B32" s="21"/>
       <c r="C32" s="65"/>
@@ -2667,7 +2667,7 @@
       <c r="G32" s="65"/>
       <c r="H32" s="65"/>
     </row>
-    <row r="33" spans="1:10" ht="18.5" thickBot="1">
+    <row r="33" spans="1:10" ht="18.75" thickBot="1">
       <c r="A33" s="15" t="s">
         <v>60</v>
       </c>
@@ -2807,7 +2807,7 @@
       </c>
       <c r="J37" s="68"/>
     </row>
-    <row r="38" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="38" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A38" s="57" t="s">
         <v>65</v>
       </c>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="J38" s="68"/>
     </row>
-    <row r="39" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="39" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A39" s="59" t="s">
         <v>66</v>
       </c>
@@ -2863,7 +2863,7 @@
       </c>
       <c r="J39" s="68"/>
     </row>
-    <row r="40" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="40" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A40" s="57" t="s">
         <v>67</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="J40" s="68"/>
     </row>
-    <row r="41" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="41" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A41" s="59" t="s">
         <v>68</v>
       </c>
@@ -2946,7 +2946,7 @@
       </c>
       <c r="J42" s="68"/>
     </row>
-    <row r="43" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="43" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A43" s="59" t="s">
         <v>70</v>
       </c>
@@ -2974,7 +2974,7 @@
       </c>
       <c r="J43" s="68"/>
     </row>
-    <row r="44" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="44" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A44" s="57" t="s">
         <v>71</v>
       </c>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="J44" s="68"/>
     </row>
-    <row r="45" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="45" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A45" s="59" t="s">
         <v>72</v>
       </c>
@@ -3112,7 +3112,7 @@
       </c>
       <c r="J48" s="68"/>
     </row>
-    <row r="49" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="49" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A49" s="59" t="s">
         <v>76</v>
       </c>
@@ -3140,7 +3140,7 @@
       </c>
       <c r="J49" s="68"/>
     </row>
-    <row r="50" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="50" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A50" s="57" t="s">
         <v>77</v>
       </c>
@@ -3251,7 +3251,7 @@
       </c>
       <c r="J53" s="68"/>
     </row>
-    <row r="54" spans="1:10" ht="15" thickBot="1">
+    <row r="54" spans="1:10" ht="15.75" thickBot="1">
       <c r="A54" s="76" t="s">
         <v>81</v>
       </c>
@@ -3279,7 +3279,7 @@
       </c>
       <c r="J54" s="68"/>
     </row>
-    <row r="55" spans="1:10" ht="15.5" thickTop="1" thickBot="1">
+    <row r="55" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A55" s="21"/>
       <c r="B55" s="21"/>
       <c r="C55" s="66"/>
@@ -3289,7 +3289,7 @@
       <c r="G55" s="66"/>
       <c r="H55" s="66"/>
     </row>
-    <row r="56" spans="1:10" ht="18.5" thickBot="1">
+    <row r="56" spans="1:10" ht="18.75" thickBot="1">
       <c r="A56" s="15" t="s">
         <v>82</v>
       </c>
@@ -3429,7 +3429,7 @@
       </c>
       <c r="J60" s="81"/>
     </row>
-    <row r="61" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="61" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A61" s="57" t="s">
         <v>65</v>
       </c>
@@ -3457,7 +3457,7 @@
       </c>
       <c r="J61" s="81"/>
     </row>
-    <row r="62" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="62" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A62" s="59" t="s">
         <v>66</v>
       </c>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="J62" s="81"/>
     </row>
-    <row r="63" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="63" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A63" s="57" t="s">
         <v>67</v>
       </c>
@@ -3541,7 +3541,7 @@
       </c>
       <c r="J64" s="81"/>
     </row>
-    <row r="65" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="65" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A65" s="57" t="s">
         <v>70</v>
       </c>
@@ -3569,7 +3569,7 @@
       </c>
       <c r="J65" s="81"/>
     </row>
-    <row r="66" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="66" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A66" s="82" t="s">
         <v>71</v>
       </c>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="J66" s="81"/>
     </row>
-    <row r="67" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="67" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A67" s="57" t="s">
         <v>72</v>
       </c>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="J70" s="81"/>
     </row>
-    <row r="71" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="71" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A71" s="57" t="s">
         <v>76</v>
       </c>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="J71" s="81"/>
     </row>
-    <row r="72" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="72" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A72" s="83" t="s">
         <v>77</v>
       </c>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="J74" s="81"/>
     </row>
-    <row r="75" spans="1:10" ht="15" thickBot="1">
+    <row r="75" spans="1:10" ht="15.75" thickBot="1">
       <c r="A75" s="84" t="s">
         <v>81</v>
       </c>
@@ -3849,7 +3849,7 @@
       </c>
       <c r="J75" s="81"/>
     </row>
-    <row r="76" spans="1:10" ht="15" thickBot="1">
+    <row r="76" spans="1:10" ht="15.75" thickBot="1">
       <c r="A76" s="38"/>
       <c r="B76" s="39"/>
       <c r="C76" s="88"/>
@@ -3861,7 +3861,7 @@
       <c r="I76" s="88"/>
       <c r="J76" s="81"/>
     </row>
-    <row r="77" spans="1:10" ht="18.5" thickBot="1">
+    <row r="77" spans="1:10" ht="18.75" thickBot="1">
       <c r="A77" s="15" t="s">
         <v>83</v>
       </c>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="J81" s="81"/>
     </row>
-    <row r="82" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="82" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A82" s="57" t="s">
         <v>65</v>
       </c>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="J82" s="81"/>
     </row>
-    <row r="83" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="83" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A83" s="59" t="s">
         <v>66</v>
       </c>
@@ -4057,7 +4057,7 @@
       </c>
       <c r="J83" s="81"/>
     </row>
-    <row r="84" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="84" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A84" s="57" t="s">
         <v>67</v>
       </c>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="J85" s="81"/>
     </row>
-    <row r="86" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="86" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A86" s="57" t="s">
         <v>70</v>
       </c>
@@ -4141,7 +4141,7 @@
       </c>
       <c r="J86" s="81"/>
     </row>
-    <row r="87" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="87" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A87" s="82" t="s">
         <v>71</v>
       </c>
@@ -4169,7 +4169,7 @@
       </c>
       <c r="J87" s="81"/>
     </row>
-    <row r="88" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="88" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A88" s="57" t="s">
         <v>72</v>
       </c>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="J91" s="81"/>
     </row>
-    <row r="92" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="92" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A92" s="57" t="s">
         <v>76</v>
       </c>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="J92" s="81"/>
     </row>
-    <row r="93" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="93" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A93" s="83" t="s">
         <v>77</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
       <c r="J95" s="81"/>
     </row>
-    <row r="96" spans="1:10" ht="15" thickBot="1">
+    <row r="96" spans="1:10" ht="15.75" thickBot="1">
       <c r="A96" s="84" t="s">
         <v>81</v>
       </c>
@@ -4421,7 +4421,7 @@
       </c>
       <c r="J96" s="81"/>
     </row>
-    <row r="97" spans="1:10" ht="15" thickBot="1">
+    <row r="97" spans="1:10" ht="15.75" thickBot="1">
       <c r="A97" s="21"/>
       <c r="B97" s="21"/>
       <c r="C97" s="66"/>
@@ -4431,7 +4431,7 @@
       <c r="G97" s="66"/>
       <c r="H97" s="66"/>
     </row>
-    <row r="98" spans="1:10" ht="18.5" thickBot="1">
+    <row r="98" spans="1:10" ht="18.75" thickBot="1">
       <c r="A98" s="15" t="s">
         <v>84</v>
       </c>
@@ -4788,7 +4788,7 @@
       </c>
       <c r="J110" s="68"/>
     </row>
-    <row r="111" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="111" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A111" s="58" t="s">
         <v>97</v>
       </c>
@@ -4816,7 +4816,7 @@
       </c>
       <c r="J111" s="68"/>
     </row>
-    <row r="112" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="112" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A112" s="60" t="s">
         <v>98</v>
       </c>
@@ -4844,7 +4844,7 @@
       </c>
       <c r="J112" s="68"/>
     </row>
-    <row r="113" spans="1:10" s="73" customFormat="1" thickBot="1">
+    <row r="113" spans="1:10" s="73" customFormat="1" ht="15.75" thickBot="1">
       <c r="A113" s="84" t="s">
         <v>81</v>
       </c>
@@ -4872,7 +4872,7 @@
       </c>
       <c r="J113" s="68"/>
     </row>
-    <row r="114" spans="1:10" s="73" customFormat="1" ht="15" thickBot="1">
+    <row r="114" spans="1:10" s="73" customFormat="1" ht="15.75" thickBot="1">
       <c r="A114" s="58"/>
       <c r="B114" s="58"/>
       <c r="C114" s="66"/>
@@ -4884,7 +4884,7 @@
       <c r="I114"/>
       <c r="J114" s="68"/>
     </row>
-    <row r="115" spans="1:10" s="73" customFormat="1" ht="18.5" thickBot="1">
+    <row r="115" spans="1:10" s="73" customFormat="1" ht="18.75" thickBot="1">
       <c r="A115" s="15" t="s">
         <v>99</v>
       </c>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="J115" s="68"/>
     </row>
-    <row r="116" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="116" spans="1:10" s="73" customFormat="1">
       <c r="A116" s="20" t="s">
         <v>61</v>
       </c>
@@ -4968,7 +4968,7 @@
       </c>
       <c r="J117" s="92"/>
     </row>
-    <row r="118" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="118" spans="1:10" s="73" customFormat="1">
       <c r="A118" s="57" t="s">
         <v>63</v>
       </c>
@@ -4996,7 +4996,7 @@
       </c>
       <c r="J118" s="68"/>
     </row>
-    <row r="119" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="119" spans="1:10" s="73" customFormat="1">
       <c r="A119" s="59" t="s">
         <v>100</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="J119" s="68"/>
     </row>
-    <row r="120" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="120" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A120" s="57" t="s">
         <v>64</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="J124" s="68"/>
     </row>
-    <row r="125" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="125" spans="1:10" s="73" customFormat="1">
       <c r="A125" s="27" t="s">
         <v>69</v>
       </c>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="J125" s="68"/>
     </row>
-    <row r="126" spans="1:10" s="73" customFormat="1" ht="14">
+    <row r="126" spans="1:10" s="73" customFormat="1" ht="14.25">
       <c r="A126" s="57" t="s">
         <v>101</v>
       </c>
@@ -5492,7 +5492,7 @@
       </c>
       <c r="J136" s="68"/>
     </row>
-    <row r="137" spans="1:10" ht="15" thickBot="1">
+    <row r="137" spans="1:10" ht="15.75" thickBot="1">
       <c r="A137" s="93" t="s">
         <v>81</v>
       </c>
@@ -5520,7 +5520,7 @@
       </c>
       <c r="J137" s="68"/>
     </row>
-    <row r="138" spans="1:10" ht="15.5" thickTop="1" thickBot="1">
+    <row r="138" spans="1:10" ht="16.5" thickTop="1" thickBot="1">
       <c r="A138" s="21"/>
       <c r="B138" s="21"/>
       <c r="C138" s="66"/>
@@ -5531,7 +5531,7 @@
       <c r="H138" s="66"/>
       <c r="J138" s="68"/>
     </row>
-    <row r="139" spans="1:10" ht="18.5" thickBot="1">
+    <row r="139" spans="1:10" ht="18.75" thickBot="1">
       <c r="A139" s="15" t="s">
         <v>102</v>
       </c>
@@ -5938,7 +5938,7 @@
       <c r="H155" s="69"/>
       <c r="I155" s="70"/>
     </row>
-    <row r="156" spans="1:10" ht="15" thickBot="1">
+    <row r="156" spans="1:10" ht="15.75" thickBot="1">
       <c r="A156" s="38" t="s">
         <v>115</v>
       </c>
@@ -6002,12 +6002,12 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="18.5" thickBot="1">
+    <row r="1" spans="1:31" ht="18.75" thickBot="1">
       <c r="B1" s="17">
         <v>2028</v>
       </c>
@@ -6367,7 +6367,7 @@
       <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:31">
       <c r="A1" t="s">
@@ -8761,17 +8761,17 @@
   </sheetPr>
   <dimension ref="A1:AE25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:AE2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.453125" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="29">
+    <row r="1" spans="1:31" ht="30">
       <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
@@ -8871,124 +8871,94 @@
         <v>10</v>
       </c>
       <c r="B2" s="3">
-        <f>'Coal Calculations'!B9</f>
         <v>0.85</v>
       </c>
       <c r="C2" s="3">
-        <f>'Coal Calculations'!C9</f>
         <v>0.85</v>
       </c>
       <c r="D2" s="3">
-        <f>'Coal Calculations'!D9</f>
         <v>0.85</v>
       </c>
       <c r="E2" s="3">
-        <f>'Coal Calculations'!E9</f>
         <v>0.85</v>
       </c>
       <c r="F2" s="3">
-        <f>'Coal Calculations'!F9</f>
         <v>0.85</v>
       </c>
       <c r="G2" s="3">
-        <f>'Coal Calculations'!G9</f>
         <v>0.85</v>
       </c>
       <c r="H2" s="3">
-        <f>'Coal Calculations'!H9</f>
         <v>0.85</v>
       </c>
       <c r="I2" s="3">
-        <f>'Coal Calculations'!I9</f>
         <v>0.85</v>
       </c>
       <c r="J2" s="3">
-        <f>'Coal Calculations'!J9</f>
         <v>0.85</v>
       </c>
       <c r="K2" s="3">
-        <f>'Coal Calculations'!K9</f>
         <v>0.85</v>
       </c>
       <c r="L2" s="3">
-        <f>'Coal Calculations'!L9</f>
         <v>0.85</v>
       </c>
       <c r="M2" s="3">
-        <f>'Coal Calculations'!M9</f>
         <v>0.85</v>
       </c>
       <c r="N2" s="3">
-        <f>'Coal Calculations'!N9</f>
         <v>0.85</v>
       </c>
       <c r="O2" s="3">
-        <f>'Coal Calculations'!O9</f>
         <v>0.85</v>
       </c>
       <c r="P2" s="3">
-        <f>'Coal Calculations'!P9</f>
         <v>0.85</v>
       </c>
       <c r="Q2" s="3">
-        <f>'Coal Calculations'!Q9</f>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R2" s="3">
-        <f>'Coal Calculations'!R9</f>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S2" s="3">
-        <f>'Coal Calculations'!S9</f>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T2" s="3">
-        <f>'Coal Calculations'!T9</f>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U2" s="3">
-        <f>'Coal Calculations'!U9</f>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V2" s="3">
-        <f>'Coal Calculations'!V9</f>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W2" s="3">
-        <f>'Coal Calculations'!W9</f>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X2" s="3">
-        <f>'Coal Calculations'!X9</f>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y2" s="3">
-        <f>'Coal Calculations'!Y9</f>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z2" s="3">
-        <f>'Coal Calculations'!Z9</f>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA2" s="3">
-        <f>'Coal Calculations'!AA9</f>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB2" s="3">
-        <f>'Coal Calculations'!AB9</f>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC2" s="3">
-        <f>'Coal Calculations'!AC9</f>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD2" s="3">
-        <f>'Coal Calculations'!AD9</f>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE2" s="3">
-        <f>'Coal Calculations'!AE9</f>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="3" spans="1:31">
@@ -10577,63 +10547,63 @@
       </c>
       <c r="Q19" s="3">
         <f t="shared" si="0"/>
-        <v>0.72031265723109072</v>
+        <v>0.85</v>
       </c>
       <c r="R19" s="3">
         <f t="shared" si="0"/>
-        <v>0.59062531446215871</v>
+        <v>0.85</v>
       </c>
       <c r="S19" s="3">
         <f t="shared" si="0"/>
-        <v>0.4609379716932267</v>
+        <v>0.85</v>
       </c>
       <c r="T19" s="3">
         <f t="shared" si="0"/>
-        <v>0.33125062892429469</v>
+        <v>0.85</v>
       </c>
       <c r="U19" s="3">
         <f t="shared" si="0"/>
-        <v>0.20156328615530583</v>
+        <v>0.85</v>
       </c>
       <c r="V19" s="3">
         <f t="shared" si="0"/>
-        <v>0.19321882697840209</v>
+        <v>0.85</v>
       </c>
       <c r="W19" s="3">
         <f t="shared" si="0"/>
-        <v>0.18487436780148059</v>
+        <v>0.85</v>
       </c>
       <c r="X19" s="3">
         <f t="shared" si="0"/>
-        <v>0.17652990862455908</v>
+        <v>0.85</v>
       </c>
       <c r="Y19" s="3">
         <f t="shared" si="0"/>
-        <v>0.16818544944764113</v>
+        <v>0.85</v>
       </c>
       <c r="Z19" s="3">
         <f t="shared" si="0"/>
-        <v>0.15984099027071963</v>
+        <v>0.85</v>
       </c>
       <c r="AA19" s="3">
         <f t="shared" si="0"/>
-        <v>0.23406504492902513</v>
+        <v>0.85</v>
       </c>
       <c r="AB19" s="3">
         <f t="shared" si="0"/>
-        <v>0.3082890995873413</v>
+        <v>0.85</v>
       </c>
       <c r="AC19" s="3">
         <f t="shared" si="0"/>
-        <v>0.38251315424565746</v>
+        <v>0.85</v>
       </c>
       <c r="AD19" s="3">
         <f t="shared" si="0"/>
-        <v>0.45673720890397362</v>
+        <v>0.85</v>
       </c>
       <c r="AE19" s="3">
         <f t="shared" si="0"/>
-        <v>0.53096126356228979</v>
+        <v>0.85</v>
       </c>
     </row>
     <row r="20" spans="1:31">

</xml_diff>